<commit_message>
Update order of annotated plot file in derivative/manifest_expected.xlsx for test_annotate_plot.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C482B200-18A7-6348-A683-F0993C6CFCDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2FE453-7674-7146-B4DB-F8341F2D06D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,10 +481,20 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="134.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="162.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -601,7 +611,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -610,23 +620,23 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -635,23 +645,23 @@
         <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -660,18 +670,18 @@
         <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
         <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add delimiter tab to plot annotation description expected results.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2FE453-7674-7146-B4DB-F8341F2D06D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEBC456-9E59-3240-9B25-30CE7D7EA336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>filename</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>sub-002_ses-003_T_log.txt</t>
+  </si>
+  <si>
+    <t>{"version": "1.2.0", "type": "plot", "attrs": {"style": "heatmap", "delimiter": "tab"}}</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,7 +695,7 @@
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
@@ -717,7 +720,7 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Correct additional mimetypes for tab delimited plot files.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEBC456-9E59-3240-9B25-30CE7D7EA336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C6452-3B9D-DB46-B35B-39512B99660A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>filename</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>{"version": "1.2.0", "type": "plot", "attrs": {"style": "heatmap", "delimiter": "tab"}}</t>
+  </si>
+  <si>
+    <t>text/x.vnd.abi.plot+Tab-separated-values</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,7 +695,7 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>
@@ -717,7 +720,7 @@
         <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Update derivative/manifest_expected.xlsx to correct state.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84836D49-CC9D-F440-8C31-7213CE0B1BAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A922D8-2DAC-0E4A-907E-41260177B006}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>filename</t>
   </si>
@@ -37,42 +37,16 @@
     <t>isSourceOf</t>
   </si>
   <si>
+    <t>scaffold_context_info.json</t>
+  </si>
+  <si>
+    <t>application/x.vnd.abi.context-information+json</t>
+  </si>
+  <si>
+    <t>{"version": "0.2.0", "id": "sparc.science.annotation_terms"}</t>
+  </si>
+  <si>
     <t>rat_brainstem_metadata.json</t>
-  </si>
-  <si>
-    <t>application/x.vnd.abi.scaffold.meta+json</t>
-  </si>
-  <si>
-    <t>rat_brainstem_Layout1_view.json</t>
-  </si>
-  <si>
-    <t>application/x.vnd.abi.scaffold.view+json</t>
-  </si>
-  <si>
-    <t>rat_brainstem_Layout1_thumbnail.jpeg</t>
-  </si>
-  <si>
-    <t>image/x.vnd.abi.thumbnail+jpeg</t>
-  </si>
-  <si>
-    <t>scaffold_context_info.json</t>
-  </si>
-  <si>
-    <t>application/x.vnd.abi.context-information+json</t>
-  </si>
-  <si>
-    <t>{"version": "0.2.0", "id": "sparc.science.annotation_terms"}</t>
-  </si>
-  <si>
-    <t>rat_brainstem_Layout2_view.json</t>
-  </si>
-  <si>
-    <t>rat_brainstem_Layout2_thumbnail.jpeg</t>
-  </si>
-  <si>
-    <t>rat_brainstem_Layout2_view.json
-rat_brainstem_Layout1_view.json
-scaffold_context_info.json</t>
   </si>
 </sst>
 </file>
@@ -128,13 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,19 +409,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -470,79 +441,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update isSourceOf and isDerivedFrom headings.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A922D8-2DAC-0E4A-907E-41260177B006}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F46B234-3047-DD43-9FE9-09B6452BAC8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,6 @@
     <t>Supplemental JSON Metadata</t>
   </si>
   <si>
-    <t>isDerivedFrom</t>
-  </si>
-  <si>
-    <t>isSourceOf</t>
-  </si>
-  <si>
     <t>scaffold_context_info.json</t>
   </si>
   <si>
@@ -47,6 +41,12 @@
   </si>
   <si>
     <t>rat_brainstem_metadata.json</t>
+  </si>
+  <si>
+    <t>IsSourceOf</t>
+  </si>
+  <si>
+    <t>IsDerivedFrom</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -435,32 +435,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change order of columns in plot test expected answers.
</commit_message>
<xml_diff>
--- a/derivative/manifest_expected.xlsx
+++ b/derivative/manifest_expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/sparc/packages/sparc-curation-tools/tests/resources/derivative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C94D61-B3D4-1C48-B63E-93E863711C0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10453AB2-04B9-2243-BD7E-44E4FEEBBFAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,10 +525,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -625,7 +625,7 @@
       <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -636,7 +636,7 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -650,7 +650,7 @@
       <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -661,7 +661,7 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -675,7 +675,7 @@
       <c r="G12" t="s">
         <v>19</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -686,7 +686,7 @@
       <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -700,7 +700,7 @@
       <c r="G14" t="s">
         <v>30</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -711,7 +711,7 @@
       <c r="F15" t="s">
         <v>21</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -725,18 +725,18 @@
       <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>